<commit_message>
update doc and example
</commit_message>
<xml_diff>
--- a/MaxsatApp/example/examples.xlsx
+++ b/MaxsatApp/example/examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Informatyka\V semestr\Inżynieria oprogramowania II\Projekt\github\projekt_inzynieria\MaxsatApp\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2E0AA4-3229-4095-970A-8BC92E637B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A6E498-42B7-4C89-A997-DDD09E95D2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{108D3861-66B3-4C24-BFD0-EFCDBD07E57A}"/>
   </bookViews>
@@ -218,19 +218,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -239,16 +239,16 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,7 +726,7 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>36</c:v>
@@ -744,7 +744,7 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -783,7 +783,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>13</c:v>
@@ -1228,13 +1228,13 @@
                   <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>94</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1273,7 +1273,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>13</c:v>
@@ -1285,7 +1285,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>13</c:v>
@@ -1690,7 +1690,7 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7</c:v>
@@ -1717,7 +1717,7 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4698,9 +4698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B374441B-BDA0-40E1-8C23-3964F2A94208}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4746,7 +4744,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -4754,7 +4752,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -4770,7 +4768,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -4778,7 +4776,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -4802,7 +4800,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -4818,7 +4816,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -4826,7 +4824,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -4834,7 +4832,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4843,7 +4842,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4922,7 +4921,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -4933,7 +4932,7 @@
         <v>36</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4970,7 +4969,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>11</v>
@@ -4987,7 +4986,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5077,7 +5076,7 @@
         <v>93</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -5098,7 +5097,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18">
         <v>14</v>
@@ -5106,15 +5105,15 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B19">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20">
         <v>13</v>
@@ -5131,7 +5130,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5186,7 +5185,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -5258,7 +5257,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>13</v>

</xml_diff>